<commit_message>
updated 1 Apr 2018
</commit_message>
<xml_diff>
--- a/pah_wikp_combo.xlsx
+++ b/pah_wikp_combo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/dev/datasci/datasets/gunviolence/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/dev/datasci/datasets/school-shooting-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D779BF46-4D59-9E4C-AB33-92ADC5C7E2C6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E129C40B-508B-814B-A0BB-DE2D41DF38D2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1060" windowWidth="25040" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3269" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3284" uniqueCount="690">
   <si>
     <t>Date</t>
   </si>
@@ -5224,6 +5224,18 @@
   </si>
   <si>
     <t>Central Michigan University shooting: Two people shot dead over a domestic dispute.</t>
+  </si>
+  <si>
+    <t>Huffman High School.  Law enforcement originally labeled the shooting as "accidental".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAB: A disgruntled employee entered the UAB Highlands Hospital on the campus of the University of Alabama at Birmingham and shot two hospital employees, fatally wounding one, on the second floor. The perpetrator then shot and fatally wounded himself. </t>
+  </si>
+  <si>
+    <t>Great Mills</t>
+  </si>
+  <si>
+    <t>Great Mills High School: School placed on lockdown after a shooting occurred in the morning. A 17-year-old male student, armed with a handgun, shot and fatally injured a female student (with whom he had a prior relationship) and wounded a male student. The student shot himself in the head, fatally, while the school resource officer simultaneously shot at him.</t>
   </si>
 </sst>
 </file>
@@ -6118,10 +6130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J653"/>
+  <dimension ref="A1:J656"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D640" sqref="D640"/>
+    <sheetView tabSelected="1" topLeftCell="A645" workbookViewId="0">
+      <selection activeCell="K650" sqref="K650"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -22924,6 +22936,84 @@
       </c>
       <c r="J653" s="9" t="s">
         <v>685</v>
+      </c>
+    </row>
+    <row r="654" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A654" s="2">
+        <v>43166</v>
+      </c>
+      <c r="B654" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C654" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E654" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F654" s="1">
+        <v>1</v>
+      </c>
+      <c r="G654" s="1">
+        <v>2</v>
+      </c>
+      <c r="I654" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="J654" s="7" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="655" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A655" s="2">
+        <v>43173</v>
+      </c>
+      <c r="B655" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C655" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E655" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F655" s="1">
+        <v>2</v>
+      </c>
+      <c r="G655" s="1">
+        <v>1</v>
+      </c>
+      <c r="I655" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="J655" s="7" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="656" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A656" s="2">
+        <v>43179</v>
+      </c>
+      <c r="B656" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="C656" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E656" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F656" s="1">
+        <v>2</v>
+      </c>
+      <c r="G656" s="1">
+        <v>1</v>
+      </c>
+      <c r="I656" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="J656" s="8" t="s">
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -22990,6 +23080,7 @@
     <hyperlink ref="J633" r:id="rId55" location="cite_note-525" display="https://en.wikipedia.org/wiki/School_shootings_in_the_United_States - cite_note-525" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
     <hyperlink ref="J635" r:id="rId56" location="cite_note-528" display="https://en.wikipedia.org/wiki/School_shootings_in_the_United_States - cite_note-528" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
     <hyperlink ref="J649" r:id="rId57" location="cite_note-auto-545" display="https://en.wikipedia.org/wiki/School_shootings_in_the_United_States - cite_note-auto-545" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="J656" r:id="rId58" tooltip="Great Mills High School" display="https://en.wikipedia.org/wiki/Great_Mills_High_School" xr:uid="{20697313-49E8-444E-9B10-F98C747E6C58}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>